<commit_message>
Checkpoint - runs: 12 itr, need e/sect 2b a var
</commit_message>
<xml_diff>
--- a/BasicOptimization/OptimizationOutputs.xlsx
+++ b/BasicOptimization/OptimizationOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\child\Documents\Flow_Lab\Onboarding\BasicOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01160ADA-2A44-431F-A4B3-4518F2E505EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF86F72-F68C-4763-9E6E-4B2655A69D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10780" xr2:uid="{C1485F64-6EA5-4EA4-B509-FCEDE7844C97}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Jacob Child</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Thrust</t>
   </si>
   <si>
-    <t>Minimizer</t>
-  </si>
-  <si>
     <t>Iterations</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>Constraints</t>
   </si>
   <si>
-    <t>[0.02295918367346939, 3.7346938775510203]</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -85,22 +79,49 @@
     <t>Elites</t>
   </si>
   <si>
-    <t>[0.025, 4.408163265306122]</t>
-  </si>
-  <si>
     <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-13</t>
   </si>
   <si>
-    <t>[0.01683673469387755, 3.9591836734693877]</t>
-  </si>
-  <si>
     <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-14</t>
   </si>
   <si>
-    <t>[0.02295918367346939, 5.081632653061225]</t>
-  </si>
-  <si>
     <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-15</t>
+  </si>
+  <si>
+    <t>OG vals:</t>
+  </si>
+  <si>
+    <t>[0.0,0.0]</t>
+  </si>
+  <si>
+    <t>Torque= .059</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-16</t>
+  </si>
+  <si>
+    <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-17</t>
+  </si>
+  <si>
+    <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-18</t>
+  </si>
+  <si>
+    <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-19</t>
+  </si>
+  <si>
+    <t>|f(x) - f(x')| = 0.0 ≤ 1.0e-20</t>
+  </si>
+  <si>
+    <t>Thrust = 3.943</t>
+  </si>
+  <si>
+    <t>Chord</t>
+  </si>
+  <si>
+    <t>Pitch</t>
   </si>
 </sst>
 </file>
@@ -150,9 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,190 +494,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FC121E-DC48-4B57-99A5-4B79701472D9}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D5" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D6" s="2">
+        <v>5.12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.2959183673469299E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.7346938775510199</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="H6" s="2">
+        <v>12</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2">
+        <v>50</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D7" s="2">
+        <v>5.23</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4.4081632653061202</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2">
+        <v>50</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D8" s="2">
+        <v>4.99</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.68367346938775E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.9591836734693802</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D6">
-        <v>5.12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6">
+      <c r="J8" s="2">
         <v>50</v>
       </c>
-      <c r="J6">
+      <c r="K8" s="2">
         <v>0.8</v>
       </c>
-      <c r="K6">
+      <c r="L8" s="2">
         <v>0.1</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D7">
-        <v>5.23</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D9" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.2959183673469299E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5.0816326530612201</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7">
+      <c r="J9" s="2">
         <v>50</v>
       </c>
-      <c r="J7">
+      <c r="K9" s="2">
         <v>0.8</v>
       </c>
-      <c r="K7">
+      <c r="L9" s="2">
         <v>0.1</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D8">
-        <v>4.99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D10" s="2">
+        <v>3.923</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-1.4285714285714199</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="2">
         <v>50</v>
       </c>
-      <c r="J8">
+      <c r="K10" s="2">
         <v>0.8</v>
       </c>
-      <c r="K8">
+      <c r="L10" s="2">
         <v>0.1</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D9">
-        <v>5.15</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D11" s="2">
+        <v>3.84</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-9.6938775510203995E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.36734693877551</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9">
+      <c r="H11" s="2">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="2">
         <v>50</v>
       </c>
-      <c r="J9">
+      <c r="K11" s="2">
         <v>0.8</v>
       </c>
-      <c r="K9">
+      <c r="L11" s="2">
         <v>0.1</v>
       </c>
-      <c r="L9">
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D12" s="2">
+        <v>3.89</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4.5918367346938702E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-0.530612244897959</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="2">
+        <v>100</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D13" s="2">
+        <v>3.9580000000000002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8.6734693877551002E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-0.530612244897959</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D14" s="2">
+        <v>3.968</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.2959183673469299E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-1.2040816326530599</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M14" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>